<commit_message>
Kennisnet: UGM conform MUG, BSM conform MBG
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kennisnet/props/Kennisnet.xlsx
+++ b/src/main/resources/input/Kennisnet/props/Kennisnet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="313">
   <si>
     <t>Name</t>
   </si>
@@ -1095,7 +1095,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1197,6 +1197,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1499,10 +1502,10 @@
   <dimension ref="A1:V110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A70" sqref="A70:F70"/>
+      <selection pane="bottomRight" activeCell="J31" sqref="J31:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1745,16 +1748,16 @@
       <c r="Q6" s="25"/>
     </row>
     <row r="7" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="41" t="b">
+      <c r="D7" s="42" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="b">
@@ -1773,10 +1776,10 @@
       <c r="U7" s="36"/>
     </row>
     <row r="8" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
       <c r="G8" s="18"/>
       <c r="L8" s="18"/>
       <c r="M8" s="15"/>
@@ -2630,9 +2633,18 @@
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="18"/>
+      <c r="I31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G31" s="18"/>
+      <c r="J31" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="K31" s="41" t="s">
+        <v>34</v>
+      </c>
       <c r="L31" s="18"/>
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
@@ -3039,16 +3051,16 @@
       <c r="Q43" s="25"/>
     </row>
     <row r="44" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="41" t="b">
+      <c r="D44" s="42" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="1" t="b">
@@ -3070,10 +3082,10 @@
       <c r="U44" s="36"/>
     </row>
     <row r="45" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
       <c r="G45" s="18"/>
       <c r="L45" s="18"/>
       <c r="M45" s="15"/>

</xml_diff>

<commit_message>
Kennisnet: createjsonschemavariant = KennisnetBSM ingesteld
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kennisnet/props/Kennisnet.xlsx
+++ b/src/main/resources/input/Kennisnet/props/Kennisnet.xlsx
@@ -1505,7 +1505,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J31" sqref="J31:K31"/>
+      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2598,7 +2598,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="G30" s="25"/>
       <c r="H30" s="29"/>

</xml_diff>

<commit_message>
Kennisnet: Geen json schema's genereren.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kennisnet/props/Kennisnet.xlsx
+++ b/src/main/resources/input/Kennisnet/props/Kennisnet.xlsx
@@ -1095,7 +1095,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1197,6 +1197,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1748,16 +1751,16 @@
       <c r="Q6" s="25"/>
     </row>
     <row r="7" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="42" t="b">
+      <c r="D7" s="43" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="b">
@@ -1776,10 +1779,10 @@
       <c r="U7" s="36"/>
     </row>
     <row r="8" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="42"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
       <c r="G8" s="18"/>
       <c r="L8" s="18"/>
       <c r="M8" s="15"/>
@@ -2559,26 +2562,26 @@
         <v>16</v>
       </c>
       <c r="N29" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="O29" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="P29" s="26" t="s">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="O29" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="P29" s="42" t="s">
+        <v>16</v>
       </c>
       <c r="Q29" s="25"/>
-      <c r="R29" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="S29" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="T29" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="U29" s="36" t="s">
-        <v>4</v>
+      <c r="R29" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="S29" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="T29" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="U29" s="42" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.4">
@@ -3051,16 +3054,16 @@
       <c r="Q43" s="25"/>
     </row>
     <row r="44" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="42" t="s">
+      <c r="A44" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="42" t="s">
+      <c r="C44" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="42" t="b">
+      <c r="D44" s="43" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="1" t="b">
@@ -3082,10 +3085,10 @@
       <c r="U44" s="36"/>
     </row>
     <row r="45" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="42"/>
-      <c r="B45" s="42"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
       <c r="G45" s="18"/>
       <c r="L45" s="18"/>
       <c r="M45" s="15"/>

</xml_diff>

<commit_message>
Kennisnet: samengaan met configuratie van VNGR
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kennisnet/props/Kennisnet.xlsx
+++ b/src/main/resources/input/Kennisnet/props/Kennisnet.xlsx
@@ -1505,10 +1505,10 @@
   <dimension ref="A1:V110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomRight" activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3865,7 +3865,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G71" s="18"/>
       <c r="L71" s="18"/>

</xml_diff>